<commit_message>
Update Test Case: Raw Data (1).xlsx
</commit_message>
<xml_diff>
--- a/System 6 Renovation Working Files/Test Files/Raw Data (1).xlsx
+++ b/System 6 Renovation Working Files/Test Files/Raw Data (1).xlsx
@@ -10,12 +10,11 @@
     <sheet name="SG11029610" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="114">
   <si>
     <t>BEGIN</t>
   </si>
@@ -351,6 +350,12 @@
   </si>
   <si>
     <t>ahjiao@acegroup.com</t>
+  </si>
+  <si>
+    <t>Coverage Code</t>
+  </si>
+  <si>
+    <t>1680: Main Insured Only</t>
   </si>
 </sst>
 </file>
@@ -934,7 +939,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -946,8 +951,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="54" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -958,25 +970,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="54" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -1338,15 +1331,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
@@ -1354,7 +1347,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3">
@@ -1365,7 +1358,7 @@
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="3">
         <v>7</v>
       </c>
@@ -1374,675 +1367,685 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
-        <v>34</v>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
+      <c r="B4" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="3">
+      <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="10"/>
+      <c r="C6" s="3">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="3">
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
+      <c r="C7" s="3">
         <v>6</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="3">
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="3">
         <v>7</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="D8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="3">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="3">
         <v>2</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="D10" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="3">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="3">
+      <c r="D11" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="3">
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="3">
-        <v>5</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="3">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="3">
-        <v>7</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="3">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="3">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="10"/>
-      <c r="C16" s="3">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="10"/>
       <c r="C18" s="3">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
-        <v>64</v>
-      </c>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>65</v>
+        <v>6</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="3">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="3">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="3">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="3">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="3">
+        <v>13</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="3">
+        <v>14</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="3">
+        <v>15</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="3">
         <v>3</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="10"/>
-      <c r="C22" s="3">
+      <c r="D27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="3">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="3">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="3">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="3">
+        <v>7</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="3">
+        <v>8</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="3">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="3">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="3">
+        <v>12</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="3">
+        <v>14</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="3">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="3">
         <v>3</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="9" t="s">
+      <c r="D38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="3">
         <v>4</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="3">
+        <v>5</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="3">
+        <v>8</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="3">
+        <v>9</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="3">
+        <v>10</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="3">
         <v>3</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D44" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="3">
+        <v>4</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="3">
         <v>5</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="3">
-        <v>4</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="3">
         <v>6</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="3">
-        <v>5</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="3">
-        <v>8</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="3">
-        <v>10</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="3">
-        <v>12</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="3">
-        <v>13</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="3">
-        <v>14</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="3">
-        <v>15</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="3">
-        <v>3</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="3">
-        <v>4</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="3">
-        <v>5</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="3">
-        <v>6</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="3">
-        <v>7</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="3">
-        <v>8</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="3">
-        <v>10</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="3">
-        <v>11</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="3">
-        <v>12</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="3">
-        <v>14</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="3">
-        <v>4</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="3">
-        <v>3</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="3">
-        <v>4</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="3">
-        <v>5</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="3">
-        <v>8</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="3">
-        <v>9</v>
-      </c>
       <c r="D47" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="10"/>
       <c r="C48" s="3">
+        <v>7</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="3">
+        <v>8</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E49"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="3">
+        <v>9</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E50"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="3">
         <v>10</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="3">
-        <v>3</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="3">
+      <c r="D51" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="3">
+        <v>12</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E52"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="3">
+        <v>14</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E53"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="3">
+        <v>15</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E54"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="3">
+        <v>2</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E55"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="3">
         <v>4</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="3">
+      <c r="D56" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="3">
         <v>5</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="3">
+      <c r="D57" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="3">
         <v>6</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="3">
+      <c r="D58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="3">
         <v>7</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="3">
-        <v>8</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="3">
-        <v>9</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="3">
-        <v>10</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="3">
-        <v>12</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="3">
-        <v>14</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="3">
-        <v>15</v>
-      </c>
       <c r="D59" s="1" t="s">
-        <v>55</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E59"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C60" s="3">
@@ -2051,90 +2054,99 @@
       <c r="D60" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E60"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="11"/>
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
       <c r="C61" s="3">
         <v>4</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="E61"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="11"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
       <c r="C62" s="3">
         <v>5</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E62"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="11"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
       <c r="C63" s="3">
         <v>8</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E63"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="11"/>
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
       <c r="C64" s="3">
         <v>10</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="11"/>
+      <c r="E64"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
       <c r="C65" s="3">
         <v>12</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="11"/>
+      <c r="E65"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
       <c r="C66" s="3">
         <v>13</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="11"/>
+      <c r="E66"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
       <c r="C67" s="3">
         <v>14</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
-      <c r="B68" s="10"/>
+      <c r="E67"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="8"/>
       <c r="C68" s="3">
         <v>15</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="9" t="s">
+      <c r="E68"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C69" s="3">
@@ -2143,99 +2155,109 @@
       <c r="D69" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="11"/>
+      <c r="E69"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
       <c r="C70" s="3">
         <v>4</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="11"/>
+      <c r="E70"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
       <c r="C71" s="3">
         <v>5</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
-      <c r="B72" s="11"/>
+      <c r="E71"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
       <c r="C72" s="3">
         <v>6</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="11"/>
+      <c r="E72"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
       <c r="C73" s="3">
         <v>7</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
-      <c r="B74" s="11"/>
+      <c r="E73"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
       <c r="C74" s="3">
         <v>8</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
-      <c r="B75" s="11"/>
+      <c r="E74"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
       <c r="C75" s="3">
         <v>10</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
-      <c r="B76" s="11"/>
+      <c r="E75"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
       <c r="C76" s="3">
         <v>11</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="13"/>
-      <c r="B77" s="11"/>
+      <c r="E76"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
       <c r="C77" s="3">
         <v>12</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
-      <c r="B78" s="10"/>
+      <c r="E77"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="7"/>
+      <c r="B78" s="8"/>
       <c r="C78" s="3">
         <v>14</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
+      <c r="E78"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="7"/>
       <c r="B79" s="1" t="s">
         <v>24</v>
       </c>
@@ -2245,10 +2267,11 @@
       <c r="D79" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
-      <c r="B80" s="9" t="s">
+      <c r="E79"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="7"/>
+      <c r="B80" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C80" s="3">
@@ -2257,59 +2280,65 @@
       <c r="D80" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
-      <c r="B81" s="11"/>
+      <c r="E80"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
       <c r="C81" s="3">
         <v>4</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
-      <c r="B82" s="11"/>
+      <c r="E81"/>
+    </row>
+    <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
       <c r="C82" s="3">
         <v>5</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
-      <c r="B83" s="11"/>
+      <c r="E82"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
       <c r="C83" s="3">
         <v>8</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
-      <c r="B84" s="11"/>
+      <c r="E83"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
       <c r="C84" s="3">
         <v>9</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="13"/>
-      <c r="B85" s="10"/>
+      <c r="E84"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="7"/>
+      <c r="B85" s="8"/>
       <c r="C85" s="3">
         <v>10</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="E85"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="7"/>
       <c r="B86" s="1" t="s">
         <v>62</v>
       </c>
@@ -2319,672 +2348,915 @@
       <c r="D86" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
-        <v>75</v>
-      </c>
+      <c r="E86"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="7"/>
       <c r="B87" s="9" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C87" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="13"/>
-      <c r="B88" s="11"/>
+        <v>35</v>
+      </c>
+      <c r="E87"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="7"/>
+      <c r="B88" s="10"/>
       <c r="C88" s="3">
         <v>4</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="13"/>
-      <c r="B89" s="11"/>
+      <c r="D88" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E88"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="7"/>
+      <c r="B89" s="10"/>
       <c r="C89" s="3">
         <v>5</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="13"/>
-      <c r="B90" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="E89"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="7"/>
+      <c r="B90" s="10"/>
       <c r="C90" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="E90"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="8"/>
       <c r="B91" s="11"/>
       <c r="C91" s="3">
+        <v>7</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E91"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" s="3">
+        <v>3</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="3">
+        <v>4</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="3">
+        <v>5</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="7"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="3">
+        <v>8</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="3">
         <v>10</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D96" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="13"/>
-      <c r="B92" s="11"/>
-      <c r="C92" s="3">
+      <c r="E96"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="7"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="3">
         <v>12</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D97" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="13"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="3">
+      <c r="E97"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="3">
         <v>13</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="D98" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="13"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="3">
+      <c r="E98"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="7"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="3">
         <v>14</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="D99" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="13"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="3">
+      <c r="E99"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="7"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="3">
         <v>15</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="13"/>
-      <c r="B96" s="9" t="s">
+      <c r="E100"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="7"/>
+      <c r="B101" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C96" s="3">
+      <c r="C101" s="3">
         <v>3</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="13"/>
-      <c r="B97" s="11"/>
-      <c r="C97" s="3">
+      <c r="E101"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="3">
         <v>4</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="D102" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="13"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="3">
+      <c r="E102"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="7"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="3">
         <v>5</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="D103" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="13"/>
-      <c r="B99" s="11"/>
-      <c r="C99" s="3">
+      <c r="E103"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="3">
         <v>6</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D104" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="13"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="3">
+      <c r="E104"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="3">
         <v>7</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D105" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="13"/>
-      <c r="B101" s="11"/>
-      <c r="C101" s="3">
+      <c r="E105"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="3">
         <v>8</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="D106" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="13"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="3">
+      <c r="E106"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="7"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="3">
         <v>10</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="D107" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="13"/>
-      <c r="B103" s="11"/>
-      <c r="C103" s="3">
+      <c r="E107"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="3">
         <v>11</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D108" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="13"/>
-      <c r="B104" s="11"/>
-      <c r="C104" s="3">
+      <c r="E108"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="3">
         <v>12</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D109" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="13"/>
-      <c r="B105" s="10"/>
-      <c r="C105" s="3">
+      <c r="E109"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="7"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="3">
         <v>14</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="13"/>
-      <c r="B106" s="1" t="s">
+      <c r="E110"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="7"/>
+      <c r="B111" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="3">
+      <c r="C111" s="3">
         <v>4</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="13"/>
-      <c r="B107" s="9" t="s">
+      <c r="E111"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="7"/>
+      <c r="B112" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C107" s="3">
+      <c r="C112" s="3">
         <v>3</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="13"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="3">
+      <c r="E112"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="3">
         <v>4</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="D113" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="13"/>
-      <c r="B109" s="11"/>
-      <c r="C109" s="3">
+      <c r="E113"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="3">
         <v>5</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="D114" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="13"/>
-      <c r="B110" s="11"/>
-      <c r="C110" s="3">
+      <c r="E114"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="3">
         <v>8</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="D115" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="13"/>
-      <c r="B111" s="11"/>
-      <c r="C111" s="3">
+      <c r="E115"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="3">
         <v>9</v>
       </c>
-      <c r="D111" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="13"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="3">
+      <c r="E116"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="7"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="3">
         <v>10</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="D117" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
-      <c r="B113" s="1" t="s">
+      <c r="E117"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
+      <c r="B118" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C113" s="3">
+      <c r="C118" s="3">
         <v>3</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="D118" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="12" t="s">
+      <c r="E118"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B114" s="9" t="s">
+      <c r="B119" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C119" s="3">
         <v>3</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D119" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="13"/>
-      <c r="B115" s="11"/>
-      <c r="C115" s="3">
+      <c r="E119"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="3">
         <v>4</v>
       </c>
-      <c r="D115" s="2" t="s">
+      <c r="D120" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="13"/>
-      <c r="B116" s="11"/>
-      <c r="C116" s="3">
+      <c r="E120"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="7"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="3">
         <v>5</v>
       </c>
-      <c r="D116" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="13"/>
-      <c r="B117" s="11"/>
-      <c r="C117" s="3">
+      <c r="E121"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="3">
         <v>8</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="D122" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="13"/>
-      <c r="B118" s="11"/>
-      <c r="C118" s="3">
+      <c r="E122"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="3">
         <v>10</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="D123" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="13"/>
-      <c r="B119" s="11"/>
-      <c r="C119" s="3">
+      <c r="E123"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="3">
         <v>12</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="13"/>
-      <c r="B120" s="11"/>
-      <c r="C120" s="3">
+      <c r="E124"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="3">
         <v>13</v>
       </c>
-      <c r="D120" s="1" t="s">
+      <c r="D125" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="13"/>
-      <c r="B121" s="11"/>
-      <c r="C121" s="3">
+      <c r="E125"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="3">
         <v>14</v>
       </c>
-      <c r="D121" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="13"/>
-      <c r="B122" s="10"/>
-      <c r="C122" s="3">
+      <c r="E126"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="7"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="3">
         <v>15</v>
       </c>
-      <c r="D122" s="1" t="s">
+      <c r="D127" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="13"/>
-      <c r="B123" s="9" t="s">
+      <c r="E127"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="7"/>
+      <c r="B128" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C123" s="3">
+      <c r="C128" s="3">
         <v>3</v>
       </c>
-      <c r="D123" s="2" t="s">
+      <c r="D128" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="13"/>
-      <c r="B124" s="11"/>
-      <c r="C124" s="3">
+      <c r="E128"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="7"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="3">
         <v>4</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="D129" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="13"/>
-      <c r="B125" s="11"/>
-      <c r="C125" s="3">
+      <c r="E129"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="3">
         <v>5</v>
       </c>
-      <c r="D125" s="1" t="s">
+      <c r="D130" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="13"/>
-      <c r="B126" s="11"/>
-      <c r="C126" s="3">
+      <c r="E130"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="7"/>
+      <c r="B131" s="7"/>
+      <c r="C131" s="3">
         <v>6</v>
       </c>
-      <c r="D126" s="1" t="s">
+      <c r="D131" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="13"/>
-      <c r="B127" s="11"/>
-      <c r="C127" s="3">
+      <c r="E131"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="3">
         <v>7</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D132" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="13"/>
-      <c r="B128" s="11"/>
-      <c r="C128" s="3">
+      <c r="E132"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="7"/>
+      <c r="B133" s="7"/>
+      <c r="C133" s="3">
         <v>8</v>
       </c>
-      <c r="D128" s="1" t="s">
+      <c r="D133" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="13"/>
-      <c r="B129" s="11"/>
-      <c r="C129" s="3">
+      <c r="E133"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="3">
         <v>10</v>
       </c>
-      <c r="D129" s="1" t="s">
+      <c r="D134" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="13"/>
-      <c r="B130" s="11"/>
-      <c r="C130" s="3">
+      <c r="E134"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="7"/>
+      <c r="B135" s="7"/>
+      <c r="C135" s="3">
         <v>11</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="D135" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="13"/>
-      <c r="B131" s="11"/>
-      <c r="C131" s="3">
+      <c r="E135"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="C136" s="3">
         <v>12</v>
       </c>
-      <c r="D131" s="1" t="s">
+      <c r="D136" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="13"/>
-      <c r="B132" s="10"/>
-      <c r="C132" s="3">
+      <c r="E136"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="7"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="3">
         <v>14</v>
       </c>
-      <c r="D132" s="1" t="s">
+      <c r="D137" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="13"/>
-      <c r="B133" s="1" t="s">
+      <c r="E137"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="7"/>
+      <c r="B138" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C133" s="3">
+      <c r="C138" s="3">
         <v>4</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="D138" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="13"/>
-      <c r="B134" s="9" t="s">
+      <c r="E138"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="7"/>
+      <c r="B139" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C134" s="3">
+      <c r="C139" s="3">
         <v>3</v>
       </c>
-      <c r="D134" s="1" t="s">
+      <c r="D139" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="13"/>
-      <c r="B135" s="11"/>
-      <c r="C135" s="3">
+      <c r="E139"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
+      <c r="C140" s="3">
         <v>4</v>
       </c>
-      <c r="D135" s="1" t="s">
+      <c r="D140" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="13"/>
-      <c r="B136" s="11"/>
-      <c r="C136" s="3">
+      <c r="E140"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="7"/>
+      <c r="B141" s="7"/>
+      <c r="C141" s="3">
         <v>5</v>
       </c>
-      <c r="D136" s="1" t="s">
+      <c r="D141" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="13"/>
-      <c r="B137" s="11"/>
-      <c r="C137" s="3">
+      <c r="E141"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="7"/>
+      <c r="B142" s="7"/>
+      <c r="C142" s="3">
         <v>8</v>
       </c>
-      <c r="D137" s="1" t="s">
+      <c r="D142" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="13"/>
-      <c r="B138" s="11"/>
-      <c r="C138" s="3">
-        <v>9</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="13"/>
-      <c r="B139" s="10"/>
-      <c r="C139" s="3">
-        <v>10</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="13"/>
-      <c r="B140" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C140" s="3">
-        <v>3</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
-      <c r="B141" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C141" s="3">
-        <v>4</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C142" s="3">
-        <v>5</v>
-      </c>
-      <c r="D142" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E143"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="7"/>
       <c r="B144" s="8"/>
       <c r="C144" s="3">
+        <v>10</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E144"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="7"/>
+      <c r="B145" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C145" s="3">
+        <v>3</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="8"/>
+      <c r="B146" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C146" s="3">
+        <v>4</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B147" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C147" s="3">
+        <v>2</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="10"/>
+      <c r="C148" s="3">
+        <v>4</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E148" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="10"/>
+      <c r="C149" s="3">
+        <v>5</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B150" s="10"/>
+      <c r="C150" s="3">
+        <v>6</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B151" s="11"/>
+      <c r="C151" s="3">
         <v>7</v>
       </c>
-      <c r="D144" s="1" t="s">
+      <c r="D151" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B152" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C152" s="3">
+        <v>3</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B153" s="10"/>
+      <c r="C153" s="3">
+        <v>5</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B154" s="10"/>
+      <c r="C154" s="3">
+        <v>6</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B155" s="11"/>
+      <c r="C155" s="3">
+        <v>7</v>
+      </c>
+      <c r="D155" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="6" t="s">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B156" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C145" s="3">
+      <c r="C156" s="3">
+        <v>3</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E156" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B157" s="10"/>
+      <c r="C157" s="3">
         <v>5</v>
       </c>
-      <c r="D145" s="1" t="s">
+      <c r="D157" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="7"/>
-      <c r="C146" s="3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B158" s="10"/>
+      <c r="C158" s="3">
         <v>6</v>
       </c>
-      <c r="D146" s="1" t="s">
+      <c r="D158" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="8"/>
-      <c r="C147" s="3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B159" s="11"/>
+      <c r="C159" s="3">
         <v>7</v>
       </c>
-      <c r="D147" s="1" t="s">
+      <c r="D159" s="1" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="A87:A113"/>
-    <mergeCell ref="B114:B122"/>
-    <mergeCell ref="B123:B132"/>
-    <mergeCell ref="B134:B139"/>
-    <mergeCell ref="A114:A141"/>
-    <mergeCell ref="B87:B95"/>
-    <mergeCell ref="B96:B105"/>
-    <mergeCell ref="A23:A59"/>
+  <mergeCells count="28">
+    <mergeCell ref="B147:B151"/>
+    <mergeCell ref="B152:B155"/>
+    <mergeCell ref="B156:B159"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B55:B59"/>
     <mergeCell ref="B60:B68"/>
     <mergeCell ref="B69:B78"/>
     <mergeCell ref="B80:B85"/>
-    <mergeCell ref="A60:A86"/>
-    <mergeCell ref="B23:B31"/>
-    <mergeCell ref="B32:B41"/>
-    <mergeCell ref="B43:B48"/>
-    <mergeCell ref="B50:B59"/>
-    <mergeCell ref="B142:B144"/>
-    <mergeCell ref="B145:B147"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B107:B112"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="B92:B100"/>
+    <mergeCell ref="B18:B26"/>
+    <mergeCell ref="B27:B36"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="B45:B54"/>
+    <mergeCell ref="A18:A59"/>
+    <mergeCell ref="A60:A91"/>
+    <mergeCell ref="A92:A118"/>
+    <mergeCell ref="B101:B110"/>
+    <mergeCell ref="B112:B117"/>
+    <mergeCell ref="A119:A146"/>
+    <mergeCell ref="B119:B127"/>
+    <mergeCell ref="B128:B137"/>
+    <mergeCell ref="B139:B144"/>
   </mergeCells>
+  <dataValidations count="17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E155:XFD155 E159:XFD159">
+      <formula1>"100838: Goodhealth Premium,100612: Incorrect Date Of Birth,100619: Incorrect Prem (at Conversion),100773: Incorrect Prem (PM vs Mkt Mat),100766: Incorrect Rating Factor,100484: Incorrect Sex Code Used,0: None,100491: Staff Premium,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E152:XFD152 E156:XFD156">
+      <formula1>"1681: Main Insured and Spouse,1680: Main Insured Only,1683: Spouse Only,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E146:XFD146">
+      <formula1>"100689: 3rdContact,216: Beneficiary,100588: Brother,210: Daughter,211: Dependent,212: Father,101070: Father-In-Law,100978: friend,207: Husband,213: Mother,100662: Mother-In-Law,100584: Nephew,100764: Niece,217: Policy Holder,100836: relative,100826: Sister,101101: Sister-In-Law,209: Son,214: Spouse,215: Unknown,208: Wife,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E56:XFD56 E88:XFD88 F148:XFD148">
+      <formula1>"1993: E-Mail,0: None,1994: Print,1995: Print Preview,1807: Test Print Output,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E46:XFD46">
+      <formula1>"873: Annual,877: Monthly,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E45:XFD45">
+      <formula1>"882: Credit Card Billing,884: Direct Billing,886: GIRO,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E43:XFD43 E144:XFD144 E117:XFD117 E85:XFD85">
+      <formula1>"100641: Divorced,101131: Married,100480: Others,100861: Separated,100724: Single,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E42:XFD42 E143:XFD143 E116:XFD116 E84:XFD84">
+      <formula1>"1002173: Administrative &amp; Support,1002140: Advertising,1002142: Aerospace/Aviation,1002143: Airlines,1002141: Architect,1002164: Arts &amp; Entertainment,1002156: Arts/Entertainment/Media,1002144: Athletics/Sports,1002165: Automobile/Transportation,1002135: Banking &amp; Finance,1002145: Biotechnology,1002146: Building &amp; Construction,1002166: Business,1002181: Chemicals,1002167: Consulting,1002162: Education,1002147: Electronics,1002158: Energy/Mining/Oil &amp; Gas,1002148: Engineering,1002150: F&amp;B,1002149: Fashion,1002151: Freight Forwarding/Delivery,1002137: Government,1002153: Healthcare/Medical,1002152: Hotel &amp; Restaurant,1002174: Human Resources,1002154: Information Technology/Multimedia,1002168: Insurance,1002169: Law/Legal,1002180: Leisure/Recreation,1002155: Manufacturing,1002175: Marine,1002138: Military,1002157: Models/Singers/Musicians,1002178: Not Applicable,1002179: Optometry,1002172: Others,1002159: Property/Real Estate,1002176: Religion,1002177: Research &amp; Development,1002160: Retail &amp; Services,1002170: Sales &amp; Marketing,1002139: Singapore Police Force,1002161: Social &amp; Community Services,1002171: Telecommunication,1002163: Tourism,1002136: Transportation,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E40:XFD40 E141:XFD141 E114:XFD114 E82:XFD82">
+      <formula1>"100652: Caucasian,100512: Chinese,100795: Eurasian,101135: Indian,100658: Japanese,100859: Malay,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E39:XFD39 E140:XFD140 E113:XFD113 E81:XFD81">
+      <formula1>"100944: American,101010: Australian,100864: British,100794: Bruneian,100531: Burmese,100525: French,101073: Hongkongers,100518: Indonesian,100657: Japanese,101008: Korean,100564: Malaysian,100691: New Zealander,100483: Others,100934: Singaporean,100869: Taiwanese,100520: Thai,101006: Vietnamese,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E38:XFD38 E139:XFD139 E112:XFD112 E80:XFD80">
+      <formula1>"100598: AM,100992: Not Applicable,101084: PM,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E37:XFD37 E111:XFD111 E79:XFD79 E148 F138:XFD138">
+      <formula1>"100895: Email,219: Home,220: Mail,100875: Property,100968: Temphome,100830: Tempwork,100785: Vacation,221: Work,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E33:XFD33 E134:XFD134 E107:XFD107 E75:XFD75">
+      <formula1>"88: Afghanistan,2459: ALAND ISLANDS,90: Albania,2460: ALGERIA,2461: AMERICAN SAMOA,2462: ANDORRA,91: Angola,2463: ANGUILLA,2464: ANTARCTICA,89: Antigua,92: Argentina,2465: ARMENIA,2466: ARUBA,100706: Asean,101111: Asia,94: Australia,93: Austria,2467: AZERBAIJAN,2468: BAHAMAS,2469: BAHRAIN,101034: Bahrain,95: Bangladesh,2470: BARBADOS,2471: BELARUS,96: Belgium,2472: BELIZE,2473: BENIN,2474: BERMUDA,2475: BHUTAN,100587: Bhutan,98: Bolivia,2476: BONAIRE, SINT EUSTATIUS AND SABA,2477: BOSNIA AND HERZEGOVINA,2478: BOTSWANA,2479: BOUVET ISLAND,101: Brazil,2480: BRITISH INDIAN OCEAN TERRITORY,99: Brunei,100: Bulgaria,2481: BURKINA FASO,97: Burma,2482: BURUNDI,104: Cambodia,2483: CAMEROON,102: Canada,2484: CAPE VERDE,100711: Caribbean,2485: CAYMAN ISLANDS,2486: CENTRAL AFRICAN REPUBLIC,2487: CHAD,103: Chile,105: China,2488: CHRISTMAS ISLAND,2489: COCOS (KEELING) ISLANDS,106: Colombia,2490: COMOROS,2491: CONGO,2492: CONGO, THE DEMOCRATIC REPUBLIC OF THE,2493: COOK ISLANDS,107: Costa Rica,2494: COTE D'IVOIRE,2495: CROATIA,108: Cuba,2496: CURACAO,109: Cyprus,110: Czech Republic,100710: Czech Republic,111: Denmark,2497: DJIBOUTI,2498: DOMINICA,112: Dominican Rp,113: Ecuador,114: Egypt,115: El Salvador,2499: EQUATORIAL GUINEA,2500: ERITREA,2501: ESTONIA,116: Ethiopia,100609: Europe,2502: FALKLAND ISLANDS (MALVINAS),2503: FAROE ISLANDS,2504: FIJI,100705: Fiji,117: Finland,2626: Former Yugoslav Republic of Macedonia,118: France,2505: FRENCH GUIANA,2506: FRENCH POLYNESIA,2507: FRENCH SOUTHERN TERRITORIES,2508: GABON,119: Gambia,2509: GEORGIA,120: Germany,121: Ghana,2510: GIBRALTAR,122: Greece,2511: GREENLAND,2512: GRENADA,2513: GUADELOUPE,2514: GUAM,100832: Guam,123: Guatemala,2515: GUERNSEY,124: Guinea,2516: GUINEA-BISSAU,125: Guyana,126: Haiti,2517: HEARD ISLAND AND MCDONALD ISLANDS,2518: HOLY SEE (VATICAN CITY STATE),87: Home Office,128: Honduras,127: Hong Kong,129: Hungary,131: Iceland,132: India,133: Indonesia,130: Iran,134: Iraq,135: Ireland,2519: ISLE OF MAN,136: Israel,137: Italy,138: Jamaica,140: Japan,2520: JERSEY,139: Jordan,2521: KAZAKHSTAN,141: Kenya,2522: KIRIBATI,142: Korea,143: Kuwait,2523: KYRGYZSTAN,2524: LAO PEOPLE'S DEMOCRATIC REPUBLIC,100486: Laos,144: LARO,148: LARO Fac-Re,2525: LATVIA,146: Lebanon,2526: LESOTHO,147: Liberia,145: Libya,2527: LIECHTENSTEIN,2528: LITHUANIA,149: Luxembourg,151: Macau,152: Madagasca,154: Malawi,150: Malaysia,2529: MALDIVES,100489: Maldives,2530: MALI,100986: Mali,157: Malta,2531: MARSHALL ISLANDS,2532: MARTINIQUE,2533: MAURITANIA,158: Mauritius,2534: MAYOTTE,159: Mexico,2535: MICRONESIA, FEDERATED STATES OF,153: Middle East,2536: MOLDOVA, REPUBLIC OF,2537: MONACO,155: Mongolia,2538: MONTENEGRO,2539: MONTSERRAT,156: Morocco,160: Mozambique,2540: MYANMAR,100761: Myanmar,2541: NAMIBIA,2542: NAURU,164: Nepal,161: Netherlands,2543: NEW CALEDONIA,166: New Zealand,163: Nicaragua,2544: NIGER,162: Nigeria,2545: NIUE,2546: NORFOLK ISLAND,2547: NORTHERN MARIANA ISLANDS,165: Norway,2548: OMAN,171: Pakistan,2549: PALAU,2550: PALESTINIAN TERRITORY, OCCUPIED,167: Panama,172: Papua New Gn,169: Paraguay,168: Peru,170: Philippines,2551: PITCAIRN,173: Poland,175: Portugal,174: Puerto Rico,2552: QATAR,100540: Regional,2553: REUNION,176: Romania,197: Russia,2554: RWANDA,2555: SAINT BARTHELEMY,2556: SAINT HELENA, ASCENSION AND TRISTAN DA CUNHA,2557: SAINT KITTS AND NEVIS,2558: SAINT LUCIA,2559: SAINT MARTIN (FRENCH PART),2560: SAINT PIERRE AND MIQUELON,2561: SAINT VINCENT AND THE GRENADINES,2562: SAMOA,2563: SAN MARINO,2564: SAO TOME AND PRINCIPE,178: Saudi Arabia,2565: SENEGAL,2566: SERBIA,179: Seychelles,181: Sierra Leone,180: Singapore,2567: SINT MAARTEN (DUTCH PART),2568: SLOVAKIA,2569: SLOVENIA,2570: SOLOMON ISLANDS,2571: SOMALIA,177: South Africa,101115: South East Asia,2572: SOUTH GEORGIA AND THE SOUTH SANDWICH ISLANDS,183: Spain,184: Sri Lanka,185: Sudan,182: Surinam,2573: SVALBARD AND JAN MAYEN,2574: SWAZILAND,186: Sweden,188: Switzerland,187: Syria,194: Taiwan,2575: TAJIKISTAN,189: Tanzania,190: Thailand,100781: Tibet,2576: TIMOR-LESTE,2577: TOGO,2578: TOKELAU,192: Tonga,2579: TRINIDAD AND TOBAGO,193: Tunisia,191: Turkey,2580: TURKMENISTAN,2581: TURKS AND CAICOS ISLANDS,2582: TUVALU,195: Uganda,2583: UKRAINE,2584: UNITED ARAB EMIRATES,100629: United Arab Emirates,196: United Kingdom,2585: UNITED STATES MINOR OUTLYING ISLANDS,199: Uruguay,200: US Virgin Islands,198: USA,2586: UZBEKISTAN,2587: VANUATU,202: Venezuela,201: Vietnam,2588: VIRGIN ISLANDS, BRITISH,2589: WALLIS AND FUTUNA,2590: WESTERN SAHARA,100493: Worldwide,100541: Worldwide excl USA/Canada,2591: YEMEN,203: Yugoslavia,204: Zaire,206: Zambia,205: Zimbabwe,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E24:XFD24 E125:XFD125 E98:XFD98 E66:XFD66">
+      <formula1>"600000: Female,600001: Male,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E21:XFD21 E122:XFD122 E95:XFD95 E63:XFD63">
+      <formula1>"100995: Dr,100728: Mdm,100519: Miss,100855: Mr,100858: Mrs,100516: Ms,100568: Prof,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E5:XFD7">
+      <formula1>"101094: Awaiting cancellation,1410: Awaiting Customer GIRO Form,1407: Awaiting GIRO/DDA Approval,1406: Batch Assigned - Poss. Miss,1409: Bounceback,1414: Campaign Suspension,1408: Data Incomplete,1412: General Policy Hold,1415: Lapsation - 2+ Months Unpaid,1411: Missing Required Data Elements,1416: New Registration - AutoSuspend,1417: Premium Check Failed,100828: ROP maturity,1413: Security Hold,100831: SPACE/Bot upload-retn f chking,100802: U/W Pend Indemnity Approval,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="E3:XFD3">
+      <formula1>"2052: Bill immediately,2051: Bill immediately and reconcile to Paid,2050: Do not bill immediately,"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E30" r:id="rId1"/>
+    <hyperlink ref="E25" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>